<commit_message>
encoding of Hero upgrade costs DONE
</commit_message>
<xml_diff>
--- a/Money-in-FVD.xlsx
+++ b/Money-in-FVD.xlsx
@@ -116,9 +116,6 @@
     <t>18 (multiple)</t>
   </si>
   <si>
-    <t>25 (stun per attack)</t>
-  </si>
-  <si>
     <t>10 (DPS)</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>12 (3 heroes at a time)</t>
+  </si>
+  <si>
+    <t>25 (stun)</t>
   </si>
 </sst>
 </file>
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="K119" sqref="K119"/>
+    <sheetView tabSelected="1" topLeftCell="B182" workbookViewId="0">
+      <selection activeCell="I188" sqref="I188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -810,7 +810,7 @@
         <v>23</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -995,7 +995,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M12" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N12" s="15">
         <f>SUM(N11,N8,N5)</f>
@@ -1185,7 +1185,7 @@
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="M23" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N23" s="15">
         <f>SUM(N22,N19,N16)</f>
@@ -1378,7 +1378,7 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="M34" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N34" s="15">
         <f>SUM(N33,N30:N31,N31,N27)</f>
@@ -1571,7 +1571,7 @@
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="M45" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N45" s="15">
         <f>SUM(N44,N41,N38)</f>
@@ -1764,7 +1764,7 @@
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="M56" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N56" s="15">
         <f>SUM(N55,N52,N49)</f>
@@ -1957,7 +1957,7 @@
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="M67" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N67" s="15">
         <f>SUM(N66,N63,N60)</f>
@@ -2150,7 +2150,7 @@
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="M78" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N78" s="15">
         <f>SUM(N77,N74,N71)</f>
@@ -2343,7 +2343,7 @@
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="M89" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N89" s="15">
         <f>SUM(N88,N85,N82)</f>
@@ -2364,7 +2364,7 @@
         <v>11</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C92" s="4">
         <v>12</v>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M100" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N100" s="15">
         <f>SUM(N99,N96,N93)</f>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M113" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N113" s="15">
         <f>SUM(N112,N109,N106)</f>
@@ -2748,7 +2748,7 @@
         <v>11</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C116" s="4">
         <v>15</v>
@@ -2919,7 +2919,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M124" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N124" s="15">
         <f>SUM(N123,N120,N117)</f>
@@ -2937,7 +2937,7 @@
         <v>11</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C127" s="4">
         <v>13</v>
@@ -3108,7 +3108,7 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M135" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N135" s="15">
         <f>SUM(N134,N131,N128)</f>
@@ -3297,7 +3297,7 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M146" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N146" s="15">
         <f>SUM(N145,N142,N139)</f>
@@ -3315,7 +3315,7 @@
         <v>11</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C149" s="4">
         <v>28</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M157" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N157" s="15">
         <f>SUM(N156,N153,N150)</f>
@@ -3504,7 +3504,7 @@
         <v>11</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C160" s="4">
         <v>13</v>
@@ -3675,7 +3675,7 @@
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M168" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N168" s="15">
         <f>SUM(N167,N164,N161)</f>
@@ -3693,7 +3693,7 @@
         <v>11</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C171" s="4">
         <v>15</v>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M179" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N179" s="15">
         <f>SUM(N178,N175,N172)</f>
@@ -3882,7 +3882,7 @@
         <v>11</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C182" s="4">
         <v>21</v>
@@ -4053,7 +4053,7 @@
     </row>
     <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M190" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N190" s="15">
         <f>SUM(N189,N186,N183)</f>
@@ -4063,10 +4063,10 @@
     <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="L192" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M192" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N192" s="15">
         <f>SUM(N190,N179,N168,N157,N146,N135,N124,N113,N100,N89,N78,N67,N56,N45,N34,N23,N12)</f>
@@ -4161,18 +4161,18 @@
   <sheetData>
     <row r="1" spans="1:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="10">
         <v>250</v>
@@ -4180,10 +4180,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="10">
         <v>300</v>
@@ -4191,10 +4191,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="10">
         <v>425</v>
@@ -4202,10 +4202,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="10">
         <v>650</v>
@@ -4213,10 +4213,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="10">
         <v>850</v>
@@ -4224,10 +4224,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="10">
         <v>1000</v>
@@ -4235,10 +4235,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="10">
         <v>1250</v>
@@ -4246,10 +4246,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="10">
         <v>1500</v>
@@ -4257,10 +4257,10 @@
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="13">
         <f>SUM(C3:C10)</f>
@@ -4269,71 +4269,71 @@
     </row>
     <row r="13" spans="1:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="10">
         <v>500</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="10">
         <v>1000</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="10">
         <v>1500</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="10">
         <v>2000</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="13">
         <f>SUM(C15:C18)</f>
@@ -4363,10 +4363,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4374,7 +4374,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1">
         <v>250</v>
@@ -4382,7 +4382,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1">
         <v>250</v>
@@ -4390,7 +4390,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1">
         <v>250</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1">
         <v>500</v>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1">
         <v>500</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1">
         <v>500</v>
@@ -4428,7 +4428,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1">
         <v>750</v>
@@ -4436,7 +4436,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1">
         <v>750</v>
@@ -4444,7 +4444,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1">
         <v>750</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1">
         <v>1000</v>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1">
         <v>1000</v>
@@ -4471,7 +4471,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1">
         <v>1000</v>
@@ -4482,7 +4482,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1">
         <v>1250</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1">
         <v>1250</v>
@@ -4498,7 +4498,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="1">
         <v>1250</v>
@@ -4509,7 +4509,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1">
         <v>1500</v>
@@ -4517,7 +4517,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="1">
         <v>1500</v>
@@ -4525,7 +4525,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" s="1">
         <v>1500</v>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1">
         <v>1750</v>
@@ -4544,7 +4544,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="1">
         <v>1750</v>
@@ -4552,7 +4552,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1">
         <v>1750</v>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1">
         <v>2000</v>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="1">
         <v>2000</v>
@@ -4579,7 +4579,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33" s="1">
         <v>2000</v>
@@ -4590,7 +4590,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1">
         <v>2250</v>
@@ -4598,7 +4598,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1">
         <v>2250</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1">
         <v>2250</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" s="1">
         <v>2750</v>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" s="1">
         <v>2750</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C41" s="1">
         <v>2750</v>
@@ -4641,10 +4641,10 @@
     </row>
     <row r="43" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" s="15">
         <f>SUM(C39:C41,C35:C37,C31:C33,C27:C29,C23:C25,C19:C21,C15:C17,C11:C13,C7:C9,C3:C5)</f>
@@ -4673,7 +4673,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="10">
         <v>42000</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="10">
         <v>42000</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="10">
         <v>5000</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="10">
         <v>6225</v>
@@ -4705,12 +4705,12 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="10">
         <v>6240</v>
@@ -4741,7 +4741,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4810,7 +4810,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="10">
         <f>SUM(B3:B10)</f>
@@ -4840,15 +4840,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unlock hero & SE cost encode DONE
</commit_message>
<xml_diff>
--- a/Money-in-FVD.xlsx
+++ b/Money-in-FVD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COSTS" sheetId="1" r:id="rId1"/>
@@ -164,18 +164,6 @@
     <t>Potions</t>
   </si>
   <si>
-    <t>Potion 1</t>
-  </si>
-  <si>
-    <t>Potion 2</t>
-  </si>
-  <si>
-    <t>Potion 3</t>
-  </si>
-  <si>
-    <t>Potion 4</t>
-  </si>
-  <si>
     <t>Level Rewards</t>
   </si>
   <si>
@@ -327,6 +315,18 @@
   </si>
   <si>
     <t>25 (stun)</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>Life Potion</t>
+  </si>
+  <si>
+    <t>Water Booster</t>
+  </si>
+  <si>
+    <t>Hero Potion</t>
   </si>
 </sst>
 </file>
@@ -789,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B182" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I188" sqref="I188"/>
     </sheetView>
   </sheetViews>
@@ -995,7 +995,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M12" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N12" s="15">
         <f>SUM(N11,N8,N5)</f>
@@ -1185,7 +1185,7 @@
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="M23" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N23" s="15">
         <f>SUM(N22,N19,N16)</f>
@@ -1378,7 +1378,7 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="M34" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N34" s="15">
         <f>SUM(N33,N30:N31,N31,N27)</f>
@@ -1571,7 +1571,7 @@
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="M45" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N45" s="15">
         <f>SUM(N44,N41,N38)</f>
@@ -1764,7 +1764,7 @@
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="M56" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N56" s="15">
         <f>SUM(N55,N52,N49)</f>
@@ -1957,7 +1957,7 @@
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="M67" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N67" s="15">
         <f>SUM(N66,N63,N60)</f>
@@ -2150,7 +2150,7 @@
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="M78" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N78" s="15">
         <f>SUM(N77,N74,N71)</f>
@@ -2343,7 +2343,7 @@
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="M89" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N89" s="15">
         <f>SUM(N88,N85,N82)</f>
@@ -2364,7 +2364,7 @@
         <v>11</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C92" s="4">
         <v>12</v>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M100" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N100" s="15">
         <f>SUM(N99,N96,N93)</f>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M113" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N113" s="15">
         <f>SUM(N112,N109,N106)</f>
@@ -2748,7 +2748,7 @@
         <v>11</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C116" s="4">
         <v>15</v>
@@ -2919,7 +2919,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M124" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N124" s="15">
         <f>SUM(N123,N120,N117)</f>
@@ -2937,7 +2937,7 @@
         <v>11</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C127" s="4">
         <v>13</v>
@@ -3108,7 +3108,7 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M135" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N135" s="15">
         <f>SUM(N134,N131,N128)</f>
@@ -3297,7 +3297,7 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M146" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N146" s="15">
         <f>SUM(N145,N142,N139)</f>
@@ -3315,7 +3315,7 @@
         <v>11</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C149" s="4">
         <v>28</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M157" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N157" s="15">
         <f>SUM(N156,N153,N150)</f>
@@ -3675,7 +3675,7 @@
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M168" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N168" s="15">
         <f>SUM(N167,N164,N161)</f>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M179" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N179" s="15">
         <f>SUM(N178,N175,N172)</f>
@@ -4053,7 +4053,7 @@
     </row>
     <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M190" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N190" s="15">
         <f>SUM(N189,N186,N183)</f>
@@ -4063,10 +4063,10 @@
     <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="L192" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="M192" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N192" s="15">
         <f>SUM(N190,N179,N168,N157,N146,N135,N124,N113,N100,N89,N78,N67,N56,N45,N34,N23,N12)</f>
@@ -4146,8 +4146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4257,7 +4257,7 @@
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>44</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>44</v>
@@ -4283,12 +4283,12 @@
         <v>500</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>44</v>
@@ -4297,12 +4297,12 @@
         <v>1000</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>44</v>
@@ -4311,12 +4311,12 @@
         <v>1500</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>44</v>
@@ -4325,12 +4325,12 @@
         <v>2000</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>44</v>
@@ -4363,10 +4363,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4374,7 +4374,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1">
         <v>250</v>
@@ -4382,7 +4382,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1">
         <v>250</v>
@@ -4390,7 +4390,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1">
         <v>250</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1">
         <v>500</v>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1">
         <v>500</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1">
         <v>500</v>
@@ -4428,7 +4428,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1">
         <v>750</v>
@@ -4436,7 +4436,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1">
         <v>750</v>
@@ -4444,7 +4444,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1">
         <v>750</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1">
         <v>1000</v>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1">
         <v>1000</v>
@@ -4471,7 +4471,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1">
         <v>1000</v>
@@ -4482,7 +4482,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1">
         <v>1250</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" s="1">
         <v>1250</v>
@@ -4498,7 +4498,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C21" s="1">
         <v>1250</v>
@@ -4509,7 +4509,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1">
         <v>1500</v>
@@ -4517,7 +4517,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C24" s="1">
         <v>1500</v>
@@ -4525,7 +4525,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1">
         <v>1500</v>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C27" s="1">
         <v>1750</v>
@@ -4544,7 +4544,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1">
         <v>1750</v>
@@ -4552,7 +4552,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1">
         <v>1750</v>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C31" s="1">
         <v>2000</v>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1">
         <v>2000</v>
@@ -4579,7 +4579,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C33" s="1">
         <v>2000</v>
@@ -4590,7 +4590,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C35" s="1">
         <v>2250</v>
@@ -4598,7 +4598,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C36" s="1">
         <v>2250</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C37" s="1">
         <v>2250</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1">
         <v>2750</v>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1">
         <v>2750</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C41" s="1">
         <v>2750</v>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="43" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>44</v>
@@ -4673,7 +4673,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B1" s="10">
         <v>42000</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B3" s="10">
         <v>42000</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B5" s="10">
         <v>5000</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B7" s="10">
         <v>6225</v>
@@ -4705,12 +4705,12 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B11" s="10">
         <v>6240</v>
@@ -4726,7 +4726,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B12" s="10">
         <f>SUM(B3:B10)</f>
@@ -4840,15 +4840,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
encoding hero HP, ATTACK, SPEED, DONE
</commit_message>
<xml_diff>
--- a/Money-in-FVD.xlsx
+++ b/Money-in-FVD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="COSTS" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="105">
   <si>
     <t>Hero Name</t>
   </si>
@@ -101,9 +101,6 @@
     <t>6 (per summon)</t>
   </si>
   <si>
-    <t>7 (DPS)</t>
-  </si>
-  <si>
     <t>4 (multiple attack)</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>overall</t>
   </si>
   <si>
-    <t>10 (singular hero) (heal)</t>
-  </si>
-  <si>
     <t>12 (3 heroes at a time)</t>
   </si>
   <si>
@@ -327,6 +321,24 @@
   </si>
   <si>
     <t>Hero Potion</t>
+  </si>
+  <si>
+    <t>can attack 3 enemies</t>
+  </si>
+  <si>
+    <t>Max: 1.5s</t>
+  </si>
+  <si>
+    <t>Damage: per 0.5s</t>
+  </si>
+  <si>
+    <t>2 mushrooms</t>
+  </si>
+  <si>
+    <t>reduces 20% speed</t>
+  </si>
+  <si>
+    <t>10 (single hero) (heal)</t>
   </si>
 </sst>
 </file>
@@ -789,15 +801,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I188" sqref="I188"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="G184" sqref="G184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="6" customWidth="1"/>
-    <col min="3" max="13" width="9.140625" style="1"/>
+    <col min="2" max="2" width="21.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="1" customWidth="1"/>
+    <col min="4" max="13" width="9.140625" style="1"/>
     <col min="14" max="14" width="18.42578125" style="9" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -810,7 +823,7 @@
         <v>23</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -995,7 +1008,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M12" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N12" s="15">
         <f>SUM(N11,N8,N5)</f>
@@ -1185,7 +1198,7 @@
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="M23" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N23" s="15">
         <f>SUM(N22,N19,N16)</f>
@@ -1378,7 +1391,7 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="M34" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N34" s="15">
         <f>SUM(N33,N30:N31,N31,N27)</f>
@@ -1392,6 +1405,9 @@
       <c r="A36" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B36" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="N36" s="9"/>
     </row>
     <row r="37" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1399,7 +1415,7 @@
         <v>11</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="4">
         <v>6</v>
@@ -1571,7 +1587,7 @@
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="M45" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N45" s="15">
         <f>SUM(N44,N41,N38)</f>
@@ -1764,7 +1780,7 @@
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="M56" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N56" s="15">
         <f>SUM(N55,N52,N49)</f>
@@ -1778,14 +1794,20 @@
       <c r="A58" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B58" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="N58" s="9"/>
     </row>
     <row r="59" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>25</v>
+      <c r="B59" s="4">
+        <v>7</v>
       </c>
       <c r="C59" s="4">
         <v>9</v>
@@ -1957,7 +1979,7 @@
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="M67" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N67" s="15">
         <f>SUM(N66,N63,N60)</f>
@@ -1971,6 +1993,9 @@
       <c r="A69" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B69" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="N69" s="9"/>
     </row>
     <row r="70" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2104,22 +2129,22 @@
         <v>13</v>
       </c>
       <c r="B76" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C76" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="D76" s="4">
         <v>2</v>
       </c>
-      <c r="C76" s="4">
+      <c r="E76" s="4">
         <v>1.9</v>
       </c>
-      <c r="D76" s="4">
+      <c r="F76" s="4">
         <v>1.8</v>
       </c>
-      <c r="E76" s="4">
-        <v>1.7</v>
-      </c>
-      <c r="F76" s="4">
+      <c r="G76" s="4">
         <v>1.6</v>
-      </c>
-      <c r="G76" s="4">
-        <v>1.5</v>
       </c>
       <c r="N76" s="9"/>
     </row>
@@ -2150,7 +2175,7 @@
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="M78" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N78" s="15">
         <f>SUM(N77,N74,N71)</f>
@@ -2164,6 +2189,9 @@
       <c r="A80" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B80" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="N80" s="9"/>
     </row>
     <row r="81" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2171,7 +2199,7 @@
         <v>11</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C81" s="4">
         <v>16</v>
@@ -2297,22 +2325,22 @@
         <v>13</v>
       </c>
       <c r="B87" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C87" s="4">
         <v>2</v>
       </c>
-      <c r="C87" s="4">
+      <c r="D87" s="4">
         <v>1.9</v>
       </c>
-      <c r="D87" s="4">
+      <c r="E87" s="4">
         <v>1.8</v>
       </c>
-      <c r="E87" s="4">
+      <c r="F87" s="4">
         <v>1.7</v>
       </c>
-      <c r="F87" s="4">
+      <c r="G87" s="4">
         <v>1.6</v>
-      </c>
-      <c r="G87" s="4">
-        <v>1.5</v>
       </c>
       <c r="N87" s="9"/>
     </row>
@@ -2343,7 +2371,7 @@
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="M89" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N89" s="15">
         <f>SUM(N88,N85,N82)</f>
@@ -2364,7 +2392,7 @@
         <v>11</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C92" s="4">
         <v>12</v>
@@ -2535,7 +2563,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M100" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N100" s="15">
         <f>SUM(N99,N96,N93)</f>
@@ -2559,7 +2587,7 @@
         <v>11</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C105" s="4">
         <v>18</v>
@@ -2685,22 +2713,22 @@
         <v>13</v>
       </c>
       <c r="B111" s="4">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="C111" s="4">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="D111" s="4">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="E111" s="4">
-        <v>2.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F111" s="4">
-        <v>2.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G111" s="4">
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="N111" s="9"/>
     </row>
@@ -2730,7 +2758,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M113" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N113" s="15">
         <f>SUM(N112,N109,N106)</f>
@@ -2748,7 +2776,7 @@
         <v>11</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C116" s="4">
         <v>15</v>
@@ -2919,7 +2947,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M124" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N124" s="15">
         <f>SUM(N123,N120,N117)</f>
@@ -2937,7 +2965,7 @@
         <v>11</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C127" s="4">
         <v>13</v>
@@ -3063,22 +3091,22 @@
         <v>13</v>
       </c>
       <c r="B133" s="4">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="C133" s="4">
-        <v>2.9</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="D133" s="4">
-        <v>2.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E133" s="4">
-        <v>2.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F133" s="4">
-        <v>2.6</v>
+        <v>2.1</v>
       </c>
       <c r="G133" s="4">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="N133" s="9"/>
     </row>
@@ -3108,7 +3136,7 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M135" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N135" s="15">
         <f>SUM(N134,N131,N128)</f>
@@ -3126,7 +3154,7 @@
         <v>11</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C138" s="4">
         <v>21</v>
@@ -3297,7 +3325,7 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M146" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N146" s="15">
         <f>SUM(N145,N142,N139)</f>
@@ -3315,7 +3343,7 @@
         <v>11</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C149" s="4">
         <v>28</v>
@@ -3486,7 +3514,7 @@
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M157" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N157" s="15">
         <f>SUM(N156,N153,N150)</f>
@@ -3504,7 +3532,7 @@
         <v>11</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C160" s="4">
         <v>13</v>
@@ -3675,7 +3703,7 @@
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M168" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N168" s="15">
         <f>SUM(N167,N164,N161)</f>
@@ -3693,7 +3721,7 @@
         <v>11</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C171" s="4">
         <v>15</v>
@@ -3864,7 +3892,7 @@
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M179" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N179" s="15">
         <f>SUM(N178,N175,N172)</f>
@@ -3882,7 +3910,7 @@
         <v>11</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C182" s="4">
         <v>21</v>
@@ -4053,7 +4081,7 @@
     </row>
     <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M190" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N190" s="15">
         <f>SUM(N189,N186,N183)</f>
@@ -4063,10 +4091,10 @@
     <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="L192" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M192" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N192" s="15">
         <f>SUM(N190,N179,N168,N157,N146,N135,N124,N113,N100,N89,N78,N67,N56,N45,N34,N23,N12)</f>
@@ -4146,7 +4174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -4161,18 +4189,18 @@
   <sheetData>
     <row r="1" spans="1:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="10">
         <v>250</v>
@@ -4180,10 +4208,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="10">
         <v>300</v>
@@ -4191,10 +4219,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="10">
         <v>425</v>
@@ -4202,10 +4230,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="10">
         <v>650</v>
@@ -4213,10 +4241,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="10">
         <v>850</v>
@@ -4224,10 +4252,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="10">
         <v>1000</v>
@@ -4235,10 +4263,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="10">
         <v>1250</v>
@@ -4246,10 +4274,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="10">
         <v>1500</v>
@@ -4257,10 +4285,10 @@
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="13">
         <f>SUM(C3:C10)</f>
@@ -4269,71 +4297,71 @@
     </row>
     <row r="13" spans="1:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="10">
         <v>500</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="10">
         <v>1000</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="10">
         <v>1500</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="10">
         <v>2000</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="13">
         <f>SUM(C15:C18)</f>
@@ -4363,10 +4391,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4374,7 +4402,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1">
         <v>250</v>
@@ -4382,7 +4410,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1">
         <v>250</v>
@@ -4390,7 +4418,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1">
         <v>250</v>
@@ -4401,7 +4429,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1">
         <v>500</v>
@@ -4409,7 +4437,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1">
         <v>500</v>
@@ -4417,7 +4445,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1">
         <v>500</v>
@@ -4428,7 +4456,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1">
         <v>750</v>
@@ -4436,7 +4464,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1">
         <v>750</v>
@@ -4444,7 +4472,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1">
         <v>750</v>
@@ -4455,7 +4483,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1">
         <v>1000</v>
@@ -4463,7 +4491,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1">
         <v>1000</v>
@@ -4471,7 +4499,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1">
         <v>1000</v>
@@ -4482,7 +4510,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1">
         <v>1250</v>
@@ -4490,7 +4518,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1">
         <v>1250</v>
@@ -4498,7 +4526,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1">
         <v>1250</v>
@@ -4509,7 +4537,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="1">
         <v>1500</v>
@@ -4517,7 +4545,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="1">
         <v>1500</v>
@@ -4525,7 +4553,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="1">
         <v>1500</v>
@@ -4536,7 +4564,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1">
         <v>1750</v>
@@ -4544,7 +4572,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="1">
         <v>1750</v>
@@ -4552,7 +4580,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1">
         <v>1750</v>
@@ -4563,7 +4591,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="1">
         <v>2000</v>
@@ -4571,7 +4599,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="1">
         <v>2000</v>
@@ -4579,7 +4607,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1">
         <v>2000</v>
@@ -4590,7 +4618,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" s="1">
         <v>2250</v>
@@ -4598,7 +4626,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="1">
         <v>2250</v>
@@ -4606,7 +4634,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="1">
         <v>2250</v>
@@ -4617,7 +4645,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="1">
         <v>2750</v>
@@ -4625,7 +4653,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" s="1">
         <v>2750</v>
@@ -4633,7 +4661,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41" s="1">
         <v>2750</v>
@@ -4641,10 +4669,10 @@
     </row>
     <row r="43" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" s="15">
         <f>SUM(C39:C41,C35:C37,C31:C33,C27:C29,C23:C25,C19:C21,C15:C17,C11:C13,C7:C9,C3:C5)</f>
@@ -4673,7 +4701,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="10">
         <v>42000</v>
@@ -4681,7 +4709,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="10">
         <v>42000</v>
@@ -4689,7 +4717,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="10">
         <v>5000</v>
@@ -4697,7 +4725,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="10">
         <v>6225</v>
@@ -4705,12 +4733,12 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="10">
         <v>6240</v>
@@ -4741,7 +4769,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4810,7 +4838,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="10">
         <f>SUM(B3:B10)</f>
@@ -4840,15 +4868,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting with the level design
</commit_message>
<xml_diff>
--- a/Money-in-FVD.xlsx
+++ b/Money-in-FVD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="108">
   <si>
     <t>Hero Name</t>
   </si>
@@ -339,6 +339,15 @@
   </si>
   <si>
     <t>10 (single hero) (heal)</t>
+  </si>
+  <si>
+    <t>Max: 1s</t>
+  </si>
+  <si>
+    <t>Damage: per 0.4s</t>
+  </si>
+  <si>
+    <t>Damage: per 0.7s</t>
   </si>
 </sst>
 </file>
@@ -801,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="G184" sqref="G184"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3525,6 +3534,12 @@
       <c r="A159" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B159" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="N159" s="9"/>
     </row>
     <row r="160" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3544,25 +3559,25 @@
         <v>19</v>
       </c>
       <c r="F160" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G160" s="4">
+        <v>22</v>
+      </c>
+      <c r="H160" s="4">
+        <v>23</v>
+      </c>
+      <c r="I160" s="4">
         <v>25</v>
       </c>
-      <c r="H160" s="4">
-        <v>29</v>
-      </c>
-      <c r="I160" s="4">
-        <v>33</v>
-      </c>
       <c r="J160" s="4">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="K160" s="4">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="L160" s="4">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="N160" s="9"/>
     </row>
@@ -3902,6 +3917,12 @@
     <row r="181" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="N181" s="9"/>
     </row>

</xml_diff>

<commit_message>
level 2 designing done
</commit_message>
<xml_diff>
--- a/Money-in-FVD.xlsx
+++ b/Money-in-FVD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="COSTS" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="109">
   <si>
     <t>Hero Name</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>Damage: per 0.7s</t>
+  </si>
+  <si>
+    <t>Initial water</t>
   </si>
 </sst>
 </file>
@@ -810,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+    <sheetView topLeftCell="A179" workbookViewId="0">
       <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
@@ -4396,10 +4399,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4407,75 +4410,97 @@
     <col min="1" max="1" width="27.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="1">
         <v>250</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="1">
         <v>250</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="1">
         <v>250</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>52</v>
       </c>
@@ -4483,7 +4508,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>53</v>
       </c>
@@ -4491,7 +4516,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>54</v>
       </c>
@@ -4499,10 +4524,10 @@
         <v>750</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>55</v>
       </c>
@@ -4510,7 +4535,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
redesign of easy levels
</commit_message>
<xml_diff>
--- a/Money-in-FVD.xlsx
+++ b/Money-in-FVD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="COSTS" sheetId="1" r:id="rId1"/>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="C181" sqref="C181"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="8">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D5" s="8">
         <v>12</v>
@@ -919,7 +919,7 @@
       </c>
       <c r="N5" s="9">
         <f>SUM(C5:L5)</f>
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="N12" s="15">
         <f>SUM(N11,N8,N5)</f>
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4122,7 +4122,7 @@
       </c>
       <c r="N192" s="15">
         <f>SUM(N190,N179,N168,N157,N146,N135,N124,N113,N100,N89,N78,N67,N56,N45,N34,N23,N12)</f>
-        <v>18785</v>
+        <v>18805</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
@@ -4401,8 +4401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4433,7 +4433,7 @@
         <v>46</v>
       </c>
       <c r="C3" s="1">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1">
         <v>380</v>
@@ -4722,7 +4722,7 @@
       </c>
       <c r="C43" s="15">
         <f>SUM(C39:C41,C35:C37,C31:C33,C27:C29,C23:C25,C19:C21,C15:C17,C11:C13,C7:C9,C3:C5)</f>
-        <v>42000</v>
+        <v>41800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stage 1 hero select module
</commit_message>
<xml_diff>
--- a/Money-in-FVD.xlsx
+++ b/Money-in-FVD.xlsx
@@ -113,9 +113,6 @@
     <t>18 (multiple)</t>
   </si>
   <si>
-    <t>10 (DPS)</t>
-  </si>
-  <si>
     <t>12 (per summon)</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>Initial water</t>
+  </si>
+  <si>
+    <t>10 (DPS)(multi)</t>
   </si>
 </sst>
 </file>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="B160" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -835,7 +835,7 @@
         <v>23</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M12" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N12" s="15">
         <f>SUM(N11,N8,N5)</f>
@@ -1210,7 +1210,7 @@
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="M23" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N23" s="15">
         <f>SUM(N22,N19,N16)</f>
@@ -1403,7 +1403,7 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="M34" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N34" s="15">
         <f>SUM(N33,N30:N31,N31,N27)</f>
@@ -1418,7 +1418,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N36" s="9"/>
     </row>
@@ -1599,7 +1599,7 @@
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="M45" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N45" s="15">
         <f>SUM(N44,N41,N38)</f>
@@ -1792,7 +1792,7 @@
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="M56" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N56" s="15">
         <f>SUM(N55,N52,N49)</f>
@@ -1807,10 +1807,10 @@
         <v>6</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N58" s="9"/>
     </row>
@@ -1991,7 +1991,7 @@
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="M67" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N67" s="15">
         <f>SUM(N66,N63,N60)</f>
@@ -2006,7 +2006,7 @@
         <v>7</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N69" s="9"/>
     </row>
@@ -2187,7 +2187,7 @@
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="M78" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N78" s="15">
         <f>SUM(N77,N74,N71)</f>
@@ -2202,7 +2202,7 @@
         <v>8</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N80" s="9"/>
     </row>
@@ -2383,7 +2383,7 @@
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="M89" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N89" s="15">
         <f>SUM(N88,N85,N82)</f>
@@ -2404,7 +2404,7 @@
         <v>11</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C92" s="4">
         <v>12</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M100" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N100" s="15">
         <f>SUM(N99,N96,N93)</f>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M113" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N113" s="15">
         <f>SUM(N112,N109,N106)</f>
@@ -2788,7 +2788,7 @@
         <v>11</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C116" s="4">
         <v>15</v>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M124" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N124" s="15">
         <f>SUM(N123,N120,N117)</f>
@@ -2977,7 +2977,7 @@
         <v>11</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C127" s="4">
         <v>13</v>
@@ -3148,7 +3148,7 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M135" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N135" s="15">
         <f>SUM(N134,N131,N128)</f>
@@ -3337,7 +3337,7 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M146" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N146" s="15">
         <f>SUM(N145,N142,N139)</f>
@@ -3355,7 +3355,7 @@
         <v>11</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C149" s="4">
         <v>28</v>
@@ -3526,7 +3526,7 @@
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M157" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N157" s="15">
         <f>SUM(N156,N153,N150)</f>
@@ -3538,10 +3538,10 @@
         <v>19</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N159" s="9"/>
     </row>
@@ -3550,7 +3550,7 @@
         <v>11</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="C160" s="4">
         <v>13</v>
@@ -3721,7 +3721,7 @@
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M168" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N168" s="15">
         <f>SUM(N167,N164,N161)</f>
@@ -3739,7 +3739,7 @@
         <v>11</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C171" s="4">
         <v>15</v>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M179" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N179" s="15">
         <f>SUM(N178,N175,N172)</f>
@@ -3922,10 +3922,10 @@
         <v>21</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N181" s="9"/>
     </row>
@@ -3934,7 +3934,7 @@
         <v>11</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C182" s="4">
         <v>21</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M190" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N190" s="15">
         <f>SUM(N189,N186,N183)</f>
@@ -4115,10 +4115,10 @@
     <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="L192" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M192" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N192" s="15">
         <f>SUM(N190,N179,N168,N157,N146,N135,N124,N113,N100,N89,N78,N67,N56,N45,N34,N23,N12)</f>
@@ -4213,18 +4213,18 @@
   <sheetData>
     <row r="1" spans="1:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="10">
         <v>250</v>
@@ -4232,10 +4232,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="10">
         <v>300</v>
@@ -4243,10 +4243,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="10">
         <v>425</v>
@@ -4254,10 +4254,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="10">
         <v>650</v>
@@ -4265,10 +4265,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="10">
         <v>850</v>
@@ -4276,10 +4276,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="10">
         <v>1000</v>
@@ -4287,10 +4287,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="10">
         <v>1250</v>
@@ -4298,10 +4298,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="10">
         <v>1500</v>
@@ -4309,10 +4309,10 @@
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="13">
         <f>SUM(C3:C10)</f>
@@ -4321,71 +4321,71 @@
     </row>
     <row r="13" spans="1:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="10">
         <v>500</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="10">
         <v>1000</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="10">
         <v>1500</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="10">
         <v>2000</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="13">
         <f>SUM(C15:C18)</f>
@@ -4416,13 +4416,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4430,7 +4430,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1">
         <v>50</v>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1">
         <v>250</v>
@@ -4452,7 +4452,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1">
         <v>250</v>
@@ -4466,7 +4466,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1">
         <v>500</v>
@@ -4477,7 +4477,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1">
         <v>500</v>
@@ -4488,7 +4488,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1">
         <v>500</v>
@@ -4502,7 +4502,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1">
         <v>750</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1">
         <v>750</v>
@@ -4518,7 +4518,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="1">
         <v>750</v>
@@ -4529,7 +4529,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1">
         <v>1000</v>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1">
         <v>1000</v>
@@ -4545,7 +4545,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1">
         <v>1000</v>
@@ -4556,7 +4556,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1">
         <v>1250</v>
@@ -4564,7 +4564,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1">
         <v>1250</v>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1">
         <v>1250</v>
@@ -4583,7 +4583,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="1">
         <v>1500</v>
@@ -4591,7 +4591,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1">
         <v>1500</v>
@@ -4599,7 +4599,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="1">
         <v>1500</v>
@@ -4610,7 +4610,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="1">
         <v>1750</v>
@@ -4618,7 +4618,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1">
         <v>1750</v>
@@ -4626,7 +4626,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="1">
         <v>1750</v>
@@ -4637,7 +4637,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" s="1">
         <v>2000</v>
@@ -4645,7 +4645,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1">
         <v>2000</v>
@@ -4653,7 +4653,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="1">
         <v>2000</v>
@@ -4664,7 +4664,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" s="1">
         <v>2250</v>
@@ -4672,7 +4672,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" s="1">
         <v>2250</v>
@@ -4680,7 +4680,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" s="1">
         <v>2250</v>
@@ -4691,7 +4691,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="1">
         <v>2750</v>
@@ -4699,7 +4699,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="1">
         <v>2750</v>
@@ -4707,7 +4707,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="1">
         <v>2750</v>
@@ -4715,10 +4715,10 @@
     </row>
     <row r="43" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="15">
         <f>SUM(C39:C41,C35:C37,C31:C33,C27:C29,C23:C25,C19:C21,C15:C17,C11:C13,C7:C9,C3:C5)</f>
@@ -4747,7 +4747,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="10">
         <v>42000</v>
@@ -4755,7 +4755,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="10">
         <v>42000</v>
@@ -4763,7 +4763,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="10">
         <v>5000</v>
@@ -4771,7 +4771,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="10">
         <v>6225</v>
@@ -4779,12 +4779,12 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="10">
         <v>6240</v>
@@ -4815,7 +4815,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4884,7 +4884,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="10">
         <f>SUM(B3:B10)</f>
@@ -4914,15 +4914,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>